<commit_message>
Revmove doubles from hiphop items bank
</commit_message>
<xml_diff>
--- a/data_raw/item_banks/hiphop_item_bank.xlsx
+++ b/data_raw/item_banks/hiphop_item_bank.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -932,7 +932,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Chuck D</t>
+          <t>Flavor Flav</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -947,7 +947,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Flavor Flav</t>
+          <t>Posdnuos</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -962,7 +962,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Posdnuos</t>
+          <t>Ice T</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -977,7 +977,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Ice T</t>
+          <t>Missy Elliot</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -992,7 +992,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Missy Elliot</t>
+          <t>Lil' Kim</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1007,7 +1007,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Lauryn Hill</t>
+          <t>Queen Latifah</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1022,7 +1022,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Lil' Kim</t>
+          <t>Salt-N-Pepa</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Queen Latifah</t>
+          <t>Foxy Brown</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1052,7 +1052,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Salt-N-Pepa</t>
+          <t>Megan Thee Stallion</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1067,7 +1067,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Foxy Brown</t>
+          <t>Cardi B</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1082,7 +1082,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Megan Thee Stallion</t>
+          <t>Little Simz</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1097,7 +1097,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Cardi B</t>
+          <t>Eve</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1112,7 +1112,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Little Simz</t>
+          <t>Doja Cat</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1127,7 +1127,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Eve</t>
+          <t>Rico Nasty</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1142,7 +1142,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Doja Cat</t>
+          <t>Da Brat</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1157,7 +1157,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Rico Nasty</t>
+          <t>Roxeanne Shanté</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1172,12 +1172,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Da Brat</t>
+          <t>Kool Herc</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>foil</t>
         </is>
       </c>
       <c r="C55">
@@ -1187,12 +1187,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Roxeanne Shanté</t>
+          <t>Premier</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>target</t>
+          <t>foil</t>
         </is>
       </c>
       <c r="C56">
@@ -1202,7 +1202,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Kool Herc</t>
+          <t>Lil Jon</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1217,7 +1217,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Premier</t>
+          <t>Grandmaster Flash</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1232,7 +1232,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Lil Jon</t>
+          <t>Grand Wizzard Theodore</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1247,7 +1247,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Grandmaster Flash</t>
+          <t>Kid Capri</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1262,7 +1262,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Grand Wizzard Theodore</t>
+          <t>Grandmaster Flowers</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1277,7 +1277,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Kid Capri</t>
+          <t>Mr. Magic</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1292,7 +1292,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Grandmaster Flowers</t>
+          <t>Jam Master Jay</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1307,7 +1307,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Mr. Magic</t>
+          <t>Funkmaster Flex</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1322,7 +1322,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Jam Master Jay</t>
+          <t>Tim Westwood</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1337,7 +1337,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Funkmaster Flex</t>
+          <t>Cosmic Kev</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1352,7 +1352,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Tim Westwood</t>
+          <t>Tony Touch</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1367,7 +1367,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Cosmic Kev</t>
+          <t>Marley Mal</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1382,7 +1382,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Tony Touch</t>
+          <t>Ron G</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1397,7 +1397,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Marley Mal</t>
+          <t>Stretch Armstrong</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1412,7 +1412,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Ron G</t>
+          <t>Jazzy Jeff</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1427,7 +1427,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Stretch Armstrong</t>
+          <t>Afrika Bambaataa</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1442,7 +1442,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Jazzy Jeff</t>
+          <t>Mister Cee</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1457,7 +1457,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Afrika Bambaataa</t>
+          <t>Easy Moe Bee</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1472,7 +1472,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Mister Cee</t>
+          <t>Tyler, the Creator</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1487,7 +1487,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Easy Moe Bee</t>
+          <t>Rick Rubin</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1502,7 +1502,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Tyler, the Creator</t>
+          <t>Roc Raida</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1517,7 +1517,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Rick Rubin</t>
+          <t>Brucie B</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1532,7 +1532,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Roc Raida</t>
+          <t>King Tech</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1547,7 +1547,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Brucie B</t>
+          <t>Chuck Chillout</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1562,7 +1562,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>King Tech</t>
+          <t>A-Trak</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1577,7 +1577,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Chuck Chillout</t>
+          <t>Pete Rock</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1592,7 +1592,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>A-Trak</t>
+          <t>Michael '5000' Watts</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1607,7 +1607,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Pete Rock</t>
+          <t>Spinderella</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1622,7 +1622,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Michael '5000' Watts</t>
+          <t>Statik Selektah</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1637,7 +1637,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Spinderella</t>
+          <t>J Dilla</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1652,7 +1652,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Statik Selektah</t>
+          <t>KayGee</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1667,7 +1667,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>J Dilla</t>
+          <t>Terminator X</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1682,7 +1682,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>KayGee</t>
+          <t>Trakgirl</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1692,36 +1692,6 @@
       </c>
       <c r="C89">
         <v>88</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>Terminator X</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>foil</t>
-        </is>
-      </c>
-      <c r="C90">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Trakgirl</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>foil</t>
-        </is>
-      </c>
-      <c r="C91">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>